<commit_message>
feat(database connection): moved over to object, more errror handling, with shipping details (#6)
</commit_message>
<xml_diff>
--- a/Database/Merch.xlsx
+++ b/Database/Merch.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="6">
   <si>
     <t>Order Id</t>
     <phoneticPr fontId="1"/>
@@ -37,35 +37,7 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>93616598-94e1-4b54-ae94-ccce8393d8bb</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>HERO-2020 HOODIES</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>S</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>XL</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>brock.tomlinson@ucalgary.ca</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>2509466196</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Brock</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Software</t>
+    <t>Shipping Details</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -370,7 +342,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E1"/>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="5" width="8.38" customWidth="1"/>
@@ -393,40 +365,6 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
-      <c r="E2">
-        <v>36.0099983215332</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3">
-        <v>10</v>
-      </c>
-      <c r="E3">
-        <v>36.0099983215332</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -435,13 +373,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F1"/>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="5" width="8.38" customWidth="1"/>
+    <col min="1" max="6" width="8.38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -457,22 +395,8 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
+      <c r="F1" t="s">
         <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(merch): initalization redone corrected database and added new fileds
</commit_message>
<xml_diff>
--- a/Database/Merch.xlsx
+++ b/Database/Merch.xlsx
@@ -15,12 +15,32 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Order Id</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>Item Id</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Size</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Quantity</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Colour</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Price</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>Email</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -78,6 +98,10 @@
   </si>
   <si>
     <t>Phone Number (shipping)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Additional Notes</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -382,13 +406,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F1"/>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="5" width="8.38" customWidth="1"/>
+    <col min="1" max="6" width="8.38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -403,6 +427,9 @@
       </c>
       <c r="E1" t="s">
         <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -413,60 +440,63 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:Q1"/>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="16" width="8.38" customWidth="1"/>
+    <col min="1" max="17" width="8.38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="H1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="I1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="J1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="K1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="L1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="M1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="N1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="O1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="P1" t="s">
-        <v>15</v>
+        <v>20</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix(merch): now writes customer info
</commit_message>
<xml_diff>
--- a/Database/Merch.xlsx
+++ b/Database/Merch.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="43">
   <si>
     <t>Order Id</t>
     <phoneticPr fontId="1"/>
@@ -102,6 +102,90 @@
   </si>
   <si>
     <t>Additional Notes</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>c0bb3a86-83e6-4aeb-ac38-5034e2793272</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Floof Hoodie</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>L</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Black</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Floof CrewNeck</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>XL</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Floof CrewNeck by Brock the One and Only Rockstar</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>brock.tomlinson@ucalgarybaja.ca</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2509466196</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Brock Tomlinson</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Software</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Yes</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t/>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Canada</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Notes</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2e61f3cd-583f-4af5-9718-486c571b54d2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>4135 University Ave NW</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>447</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Calgary</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Alberta</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>T3B 6K8</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -406,7 +490,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F23"/>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="6" width="8.38" customWidth="1"/>
@@ -432,6 +516,446 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2">
+        <v>49.9900016784668</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3">
+        <v>39.9900016784668</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4">
+        <v>39.9900016784668</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5">
+        <v>39.9900016784668</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6">
+        <v>39.9900016784668</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7">
+        <v>39.9900016784668</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8">
+        <v>39.9900016784668</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9">
+        <v>39.9900016784668</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10">
+        <v>39.9900016784668</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11">
+        <v>39.9900016784668</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12">
+        <v>39.9900016784668</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13">
+        <v>49.9900016784668</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14">
+        <v>39.9900016784668</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15">
+        <v>39.9900016784668</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16">
+        <v>39.9900016784668</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17">
+        <v>39.9900016784668</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18">
+        <v>39.9900016784668</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19">
+        <v>39.9900016784668</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20">
+        <v>39.9900016784668</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21">
+        <v>39.9900016784668</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
+        <v>25</v>
+      </c>
+      <c r="F22">
+        <v>39.9900016784668</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23">
+        <v>39.9900016784668</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -440,7 +964,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:Q3"/>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="17" width="8.38" customWidth="1"/>
@@ -499,6 +1023,106 @@
         <v>21</v>
       </c>
     </row>
+    <row r="2" spans="1:17">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2">
+        <v>472.38446044921875</v>
+      </c>
+      <c r="G2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" t="s">
+        <v>34</v>
+      </c>
+      <c r="L2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M2" t="s">
+        <v>34</v>
+      </c>
+      <c r="N2" t="s">
+        <v>35</v>
+      </c>
+      <c r="O2" t="s">
+        <v>34</v>
+      </c>
+      <c r="P2" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3">
+        <v>472.38446044921875</v>
+      </c>
+      <c r="G3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K3" t="s">
+        <v>39</v>
+      </c>
+      <c r="L3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M3" t="s">
+        <v>41</v>
+      </c>
+      <c r="N3" t="s">
+        <v>35</v>
+      </c>
+      <c r="O3" t="s">
+        <v>42</v>
+      </c>
+      <c r="P3" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
feat(get merch): naming convension
</commit_message>
<xml_diff>
--- a/Database/Merch.xlsx
+++ b/Database/Merch.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="44">
   <si>
     <t>Order Id</t>
     <phoneticPr fontId="1"/>
@@ -186,6 +186,10 @@
   </si>
   <si>
     <t>T3B 6K8</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ea52f74b-7b77-4248-9773-3898b445486d</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -490,7 +494,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F34"/>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="6" width="8.38" customWidth="1"/>
@@ -956,6 +960,226 @@
         <v>39.9900016784668</v>
       </c>
     </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24" t="s">
+        <v>25</v>
+      </c>
+      <c r="F24">
+        <v>49.9900016784668</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25" t="s">
+        <v>25</v>
+      </c>
+      <c r="F25">
+        <v>39.9900016784668</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
+        <v>25</v>
+      </c>
+      <c r="F26">
+        <v>39.9900016784668</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27" t="s">
+        <v>25</v>
+      </c>
+      <c r="F27">
+        <v>39.9900016784668</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28" t="s">
+        <v>25</v>
+      </c>
+      <c r="F28">
+        <v>39.9900016784668</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29" t="s">
+        <v>25</v>
+      </c>
+      <c r="F29">
+        <v>39.9900016784668</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30" t="s">
+        <v>25</v>
+      </c>
+      <c r="F30">
+        <v>39.9900016784668</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31" t="s">
+        <v>25</v>
+      </c>
+      <c r="F31">
+        <v>39.9900016784668</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" t="s">
+        <v>26</v>
+      </c>
+      <c r="C32" t="s">
+        <v>27</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32" t="s">
+        <v>25</v>
+      </c>
+      <c r="F32">
+        <v>39.9900016784668</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" t="s">
+        <v>27</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33" t="s">
+        <v>25</v>
+      </c>
+      <c r="F33">
+        <v>39.9900016784668</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34" t="s">
+        <v>26</v>
+      </c>
+      <c r="C34" t="s">
+        <v>27</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34" t="s">
+        <v>25</v>
+      </c>
+      <c r="F34">
+        <v>39.9900016784668</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -964,7 +1188,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:Q4"/>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="17" width="8.38" customWidth="1"/>
@@ -1123,6 +1347,56 @@
         <v>36</v>
       </c>
     </row>
+    <row r="4" spans="1:17">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4">
+        <v>472.38446044921875</v>
+      </c>
+      <c r="G4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K4" t="s">
+        <v>34</v>
+      </c>
+      <c r="L4" t="s">
+        <v>34</v>
+      </c>
+      <c r="M4" t="s">
+        <v>34</v>
+      </c>
+      <c r="N4" t="s">
+        <v>35</v>
+      </c>
+      <c r="O4" t="s">
+        <v>34</v>
+      </c>
+      <c r="P4" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>